<commit_message>
Atualiza├º├úo autom├ítica KPIs + Pre├ºo M├®dio
</commit_message>
<xml_diff>
--- a/excel/PEDIDOS_2026.xlsx
+++ b/excel/PEDIDOS_2026.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USUARIOS\ADM05\Documents\dashboard_tv\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F926CFF3-AC41-4B1C-BD7B-7AC95910344E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F31A60C-5592-4643-B8B2-D93D6810B5A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" xr2:uid="{C1828F10-D84A-418A-AAF0-1B51BFAF300A}"/>
   </bookViews>
@@ -1092,11 +1092,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5695F443-BC3D-48D0-8CD1-D8C4D00277A1}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AU1843"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:AU197"/>
+      <pane ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E167" sqref="E167:E197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1292,7 +1293,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1420,7 +1421,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -1500,7 +1501,7 @@
       <c r="AE3" s="3"/>
       <c r="AK3" s="5"/>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -1562,7 +1563,7 @@
       <c r="AE4" s="3"/>
       <c r="AK4" s="5"/>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -1690,7 +1691,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -1770,7 +1771,7 @@
       <c r="AE6" s="3"/>
       <c r="AK6" s="5"/>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>63</v>
       </c>
@@ -1830,7 +1831,7 @@
       <c r="AE7" s="3"/>
       <c r="AK7" s="5"/>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -1955,7 +1956,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -2083,7 +2084,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -2211,7 +2212,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>81</v>
       </c>
@@ -2291,7 +2292,7 @@
       <c r="AE11" s="3"/>
       <c r="AK11" s="5"/>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>63</v>
       </c>
@@ -2352,7 +2353,7 @@
       <c r="AE12" s="3"/>
       <c r="AK12" s="5"/>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>81</v>
       </c>
@@ -2427,7 +2428,7 @@
       </c>
       <c r="AK13" s="5"/>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -2486,7 +2487,7 @@
       <c r="AE14" s="3"/>
       <c r="AK14" s="5"/>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -2569,7 +2570,7 @@
       <c r="AE15" s="3"/>
       <c r="AK15" s="5"/>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -2630,7 +2631,7 @@
       <c r="AE16" s="3"/>
       <c r="AK16" s="5"/>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -2710,7 +2711,7 @@
       <c r="AE17" s="3"/>
       <c r="AK17" s="5"/>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>63</v>
       </c>
@@ -2770,7 +2771,7 @@
       <c r="AE18" s="3"/>
       <c r="AK18" s="5"/>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>96</v>
       </c>
@@ -2898,7 +2899,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -3029,7 +3030,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -3157,7 +3158,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>81</v>
       </c>
@@ -3285,7 +3286,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>81</v>
       </c>
@@ -3362,7 +3363,7 @@
       <c r="AE23" s="3"/>
       <c r="AK23" s="5"/>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>63</v>
       </c>
@@ -3419,7 +3420,7 @@
       </c>
       <c r="X24" s="4"/>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -3547,7 +3548,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -3675,7 +3676,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>47</v>
       </c>
@@ -3806,7 +3807,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>47</v>
       </c>
@@ -3885,7 +3886,7 @@
       <c r="Z28" s="3"/>
       <c r="AK28" s="5"/>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>63</v>
       </c>
@@ -3942,7 +3943,7 @@
       </c>
       <c r="X29" s="4"/>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>81</v>
       </c>
@@ -4019,7 +4020,7 @@
       <c r="AE30" s="3"/>
       <c r="AK30" s="5"/>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>63</v>
       </c>
@@ -4076,7 +4077,7 @@
       </c>
       <c r="X31" s="4"/>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>47</v>
       </c>
@@ -4201,7 +4202,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>47</v>
       </c>
@@ -4326,7 +4327,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>96</v>
       </c>
@@ -4457,7 +4458,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>96</v>
       </c>
@@ -4588,7 +4589,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>96</v>
       </c>
@@ -4719,7 +4720,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>96</v>
       </c>
@@ -4850,7 +4851,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>96</v>
       </c>
@@ -4981,7 +4982,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>96</v>
       </c>
@@ -5112,7 +5113,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>47</v>
       </c>
@@ -5240,7 +5241,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>96</v>
       </c>
@@ -5368,7 +5369,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="42" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>47</v>
       </c>
@@ -5496,7 +5497,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>47</v>
       </c>
@@ -5624,7 +5625,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>47</v>
       </c>
@@ -5752,7 +5753,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>96</v>
       </c>
@@ -5833,7 +5834,7 @@
       <c r="AE45" s="3"/>
       <c r="AK45" s="5"/>
     </row>
-    <row r="46" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>63</v>
       </c>
@@ -5897,7 +5898,7 @@
       <c r="AE46" s="3"/>
       <c r="AK46" s="5"/>
     </row>
-    <row r="47" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>96</v>
       </c>
@@ -5976,7 +5977,7 @@
       <c r="AB47" s="3"/>
       <c r="AK47" s="5"/>
     </row>
-    <row r="48" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>63</v>
       </c>
@@ -6037,7 +6038,7 @@
       <c r="X48" s="4"/>
       <c r="AK48" s="5"/>
     </row>
-    <row r="49" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -6117,7 +6118,7 @@
       <c r="AE49" s="3"/>
       <c r="AK49" s="5"/>
     </row>
-    <row r="50" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>63</v>
       </c>
@@ -6177,7 +6178,7 @@
       <c r="AE50" s="3"/>
       <c r="AK50" s="5"/>
     </row>
-    <row r="51" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>81</v>
       </c>
@@ -6305,7 +6306,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>47</v>
       </c>
@@ -6433,7 +6434,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="53" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>47</v>
       </c>
@@ -6561,7 +6562,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="54" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>47</v>
       </c>
@@ -6641,7 +6642,7 @@
       <c r="AE54" s="3"/>
       <c r="AK54" s="5"/>
     </row>
-    <row r="55" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>63</v>
       </c>
@@ -6701,7 +6702,7 @@
       <c r="AE55" s="3"/>
       <c r="AK55" s="5"/>
     </row>
-    <row r="56" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>47</v>
       </c>
@@ -6832,7 +6833,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>136</v>
       </c>
@@ -6912,7 +6913,7 @@
       <c r="AE57" s="3"/>
       <c r="AK57" s="5"/>
     </row>
-    <row r="58" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>63</v>
       </c>
@@ -6973,7 +6974,7 @@
       <c r="X58" s="4"/>
       <c r="AK58" s="5"/>
     </row>
-    <row r="59" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>47</v>
       </c>
@@ -7101,7 +7102,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>81</v>
       </c>
@@ -7229,7 +7230,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="61" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>96</v>
       </c>
@@ -7306,7 +7307,7 @@
       <c r="AE61" s="3"/>
       <c r="AK61" s="5"/>
     </row>
-    <row r="62" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>63</v>
       </c>
@@ -7370,7 +7371,7 @@
       <c r="AE62" s="3"/>
       <c r="AK62" s="5"/>
     </row>
-    <row r="63" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>96</v>
       </c>
@@ -7498,7 +7499,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="64" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>96</v>
       </c>
@@ -7626,7 +7627,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="65" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>81</v>
       </c>
@@ -7754,7 +7755,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="66" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>81</v>
       </c>
@@ -7882,7 +7883,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="67" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>81</v>
       </c>
@@ -8010,7 +8011,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="68" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>81</v>
       </c>
@@ -8138,7 +8139,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="69" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>47</v>
       </c>
@@ -8218,7 +8219,7 @@
       <c r="AE69" s="3"/>
       <c r="AK69" s="5"/>
     </row>
-    <row r="70" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>63</v>
       </c>
@@ -8278,7 +8279,7 @@
       <c r="AE70" s="3"/>
       <c r="AK70" s="5"/>
     </row>
-    <row r="71" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>47</v>
       </c>
@@ -8358,7 +8359,7 @@
       <c r="AE71" s="3"/>
       <c r="AK71" s="5"/>
     </row>
-    <row r="72" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>63</v>
       </c>
@@ -8420,7 +8421,7 @@
       <c r="AB72" s="3"/>
       <c r="AK72" s="5"/>
     </row>
-    <row r="73" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>47</v>
       </c>
@@ -8501,7 +8502,7 @@
       <c r="AE73" s="3"/>
       <c r="AK73" s="5"/>
     </row>
-    <row r="74" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>63</v>
       </c>
@@ -8565,7 +8566,7 @@
       <c r="AE74" s="3"/>
       <c r="AK74" s="5"/>
     </row>
-    <row r="75" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>47</v>
       </c>
@@ -8646,7 +8647,7 @@
       <c r="AE75" s="3"/>
       <c r="AK75" s="5"/>
     </row>
-    <row r="76" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>63</v>
       </c>
@@ -8710,7 +8711,7 @@
       <c r="AE76" s="3"/>
       <c r="AK76" s="5"/>
     </row>
-    <row r="77" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>47</v>
       </c>
@@ -8790,7 +8791,7 @@
       <c r="AE77" s="3"/>
       <c r="AK77" s="5"/>
     </row>
-    <row r="78" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>63</v>
       </c>
@@ -8853,7 +8854,7 @@
       <c r="AE78" s="3"/>
       <c r="AK78" s="5"/>
     </row>
-    <row r="79" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>96</v>
       </c>
@@ -8931,7 +8932,7 @@
       <c r="AE79" s="3"/>
       <c r="AK79" s="5"/>
     </row>
-    <row r="80" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>63</v>
       </c>
@@ -8995,7 +8996,7 @@
       <c r="AE80" s="3"/>
       <c r="AK80" s="5"/>
     </row>
-    <row r="81" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>96</v>
       </c>
@@ -9073,7 +9074,7 @@
       <c r="AE81" s="3"/>
       <c r="AK81" s="5"/>
     </row>
-    <row r="82" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>63</v>
       </c>
@@ -9138,7 +9139,7 @@
       <c r="AE82" s="3"/>
       <c r="AK82" s="5"/>
     </row>
-    <row r="83" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>47</v>
       </c>
@@ -9266,7 +9267,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="84" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>47</v>
       </c>
@@ -9394,7 +9395,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="85" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>47</v>
       </c>
@@ -9475,7 +9476,7 @@
       <c r="AE85" s="3"/>
       <c r="AK85" s="5"/>
     </row>
-    <row r="86" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>63</v>
       </c>
@@ -9533,7 +9534,7 @@
       <c r="X86" s="4"/>
       <c r="AK86" s="5"/>
     </row>
-    <row r="87" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>96</v>
       </c>
@@ -9661,7 +9662,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="88" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>96</v>
       </c>
@@ -9789,7 +9790,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="89" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>47</v>
       </c>
@@ -9920,7 +9921,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="90" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>47</v>
       </c>
@@ -10000,7 +10001,7 @@
       <c r="AE90" s="3"/>
       <c r="AK90" s="5"/>
     </row>
-    <row r="91" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>63</v>
       </c>
@@ -10063,7 +10064,7 @@
       <c r="AE91" s="3"/>
       <c r="AK91" s="5"/>
     </row>
-    <row r="92" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>96</v>
       </c>
@@ -10144,7 +10145,7 @@
       <c r="AE92" s="3"/>
       <c r="AK92" s="5"/>
     </row>
-    <row r="93" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>63</v>
       </c>
@@ -10207,7 +10208,7 @@
       <c r="AE93" s="3"/>
       <c r="AK93" s="5"/>
     </row>
-    <row r="94" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>96</v>
       </c>
@@ -10335,7 +10336,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="95" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>47</v>
       </c>
@@ -10415,7 +10416,7 @@
       <c r="AE95" s="3"/>
       <c r="AK95" s="5"/>
     </row>
-    <row r="96" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>63</v>
       </c>
@@ -10480,7 +10481,7 @@
       <c r="AE96" s="3"/>
       <c r="AK96" s="5"/>
     </row>
-    <row r="97" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>47</v>
       </c>
@@ -10605,7 +10606,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="98" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>47</v>
       </c>
@@ -10730,7 +10731,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="99" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>81</v>
       </c>
@@ -10858,7 +10859,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="100" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>47</v>
       </c>
@@ -10989,7 +10990,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="101" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>96</v>
       </c>
@@ -11120,7 +11121,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="102" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>96</v>
       </c>
@@ -11248,7 +11249,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="103" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>47</v>
       </c>
@@ -11329,7 +11330,7 @@
       <c r="AE103" s="3"/>
       <c r="AK103" s="5"/>
     </row>
-    <row r="104" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>63</v>
       </c>
@@ -11391,7 +11392,7 @@
       <c r="AE104" s="3"/>
       <c r="AK104" s="5"/>
     </row>
-    <row r="105" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>47</v>
       </c>
@@ -11516,7 +11517,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="106" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>47</v>
       </c>
@@ -11641,7 +11642,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="107" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>47</v>
       </c>
@@ -11721,7 +11722,7 @@
       <c r="AE107" s="3"/>
       <c r="AK107" s="5"/>
     </row>
-    <row r="108" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>63</v>
       </c>
@@ -11781,7 +11782,7 @@
       <c r="AE108" s="3"/>
       <c r="AK108" s="5"/>
     </row>
-    <row r="109" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>96</v>
       </c>
@@ -11909,7 +11910,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="110" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>96</v>
       </c>
@@ -12037,7 +12038,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="111" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>47</v>
       </c>
@@ -12168,7 +12169,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="112" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>47</v>
       </c>
@@ -12250,7 +12251,7 @@
       <c r="AE112" s="3"/>
       <c r="AK112" s="5"/>
     </row>
-    <row r="113" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>63</v>
       </c>
@@ -12314,7 +12315,7 @@
       <c r="AE113" s="3"/>
       <c r="AK113" s="5"/>
     </row>
-    <row r="114" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>96</v>
       </c>
@@ -12391,7 +12392,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="115" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>63</v>
       </c>
@@ -12449,7 +12450,7 @@
       <c r="X115" s="4"/>
       <c r="AK115" s="5"/>
     </row>
-    <row r="116" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>96</v>
       </c>
@@ -12580,7 +12581,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="117" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>96</v>
       </c>
@@ -12660,7 +12661,7 @@
       <c r="AE117" s="3"/>
       <c r="AK117" s="5"/>
     </row>
-    <row r="118" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>63</v>
       </c>
@@ -12724,7 +12725,7 @@
       <c r="AE118" s="3"/>
       <c r="AK118" s="5"/>
     </row>
-    <row r="119" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>96</v>
       </c>
@@ -12805,7 +12806,7 @@
       <c r="AE119" s="3"/>
       <c r="AK119" s="5"/>
     </row>
-    <row r="120" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>63</v>
       </c>
@@ -12869,7 +12870,7 @@
       <c r="AE120" s="3"/>
       <c r="AK120" s="5"/>
     </row>
-    <row r="121" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>47</v>
       </c>
@@ -12950,7 +12951,7 @@
       <c r="AE121" s="3"/>
       <c r="AK121" s="5"/>
     </row>
-    <row r="122" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>63</v>
       </c>
@@ -13011,7 +13012,7 @@
       <c r="AE122" s="3"/>
       <c r="AK122" s="5"/>
     </row>
-    <row r="123" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>47</v>
       </c>
@@ -13139,7 +13140,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="124" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>96</v>
       </c>
@@ -13270,7 +13271,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="125" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>96</v>
       </c>
@@ -13350,7 +13351,7 @@
       <c r="AE125" s="3"/>
       <c r="AK125" s="5"/>
     </row>
-    <row r="126" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>63</v>
       </c>
@@ -13410,7 +13411,7 @@
       <c r="AE126" s="3"/>
       <c r="AK126" s="5"/>
     </row>
-    <row r="127" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>47</v>
       </c>
@@ -13490,7 +13491,7 @@
       <c r="AE127" s="3"/>
       <c r="AK127" s="5"/>
     </row>
-    <row r="128" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>63</v>
       </c>
@@ -13551,7 +13552,7 @@
       <c r="AE128" s="3"/>
       <c r="AK128" s="5"/>
     </row>
-    <row r="129" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>96</v>
       </c>
@@ -13679,7 +13680,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="130" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>47</v>
       </c>
@@ -13756,7 +13757,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="131" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>63</v>
       </c>
@@ -13812,7 +13813,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="132" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>81</v>
       </c>
@@ -13889,7 +13890,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="133" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>63</v>
       </c>
@@ -13945,7 +13946,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="134" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>47</v>
       </c>
@@ -14023,7 +14024,7 @@
       </c>
       <c r="AK134" s="5"/>
     </row>
-    <row r="135" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>63</v>
       </c>
@@ -14086,7 +14087,7 @@
       <c r="AE135" s="3"/>
       <c r="AK135" s="5"/>
     </row>
-    <row r="136" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>47</v>
       </c>
@@ -14214,7 +14215,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="137" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>47</v>
       </c>
@@ -14339,7 +14340,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="138" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>47</v>
       </c>
@@ -14467,7 +14468,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="139" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>81</v>
       </c>
@@ -14545,7 +14546,7 @@
       <c r="AE139" s="3"/>
       <c r="AK139" s="5"/>
     </row>
-    <row r="140" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>63</v>
       </c>
@@ -15072,7 +15073,7 @@
       <c r="AE144" s="3"/>
       <c r="AK144" s="5"/>
     </row>
-    <row r="145" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>63</v>
       </c>
@@ -15213,7 +15214,7 @@
       <c r="AE146" s="3"/>
       <c r="AK146" s="5"/>
     </row>
-    <row r="147" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>63</v>
       </c>
@@ -15353,7 +15354,7 @@
       <c r="AE148" s="3"/>
       <c r="AK148" s="5"/>
     </row>
-    <row r="149" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>63</v>
       </c>
@@ -15494,7 +15495,7 @@
       <c r="AE150" s="3"/>
       <c r="AK150" s="5"/>
     </row>
-    <row r="151" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>63</v>
       </c>
@@ -15761,7 +15762,7 @@
       <c r="AE153" s="3"/>
       <c r="AK153" s="5"/>
     </row>
-    <row r="154" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>63</v>
       </c>
@@ -15901,7 +15902,7 @@
       <c r="AE155" s="3"/>
       <c r="AK155" s="5"/>
     </row>
-    <row r="156" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>63</v>
       </c>
@@ -16937,7 +16938,7 @@
       <c r="AE164" s="3"/>
       <c r="AK164" s="5"/>
     </row>
-    <row r="165" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>63</v>
       </c>
@@ -17467,7 +17468,7 @@
       <c r="AE169" s="3"/>
       <c r="AK169" s="5"/>
     </row>
-    <row r="170" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>63</v>
       </c>
@@ -17606,7 +17607,7 @@
       <c r="AB171" s="3"/>
       <c r="AK171" s="5"/>
     </row>
-    <row r="172" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>63</v>
       </c>
@@ -17742,7 +17743,7 @@
       <c r="AB173" s="3"/>
       <c r="AK173" s="5"/>
     </row>
-    <row r="174" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>63</v>
       </c>
@@ -17882,7 +17883,7 @@
       <c r="AB175" s="3"/>
       <c r="AK175" s="5"/>
     </row>
-    <row r="176" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>63</v>
       </c>
@@ -18016,7 +18017,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="178" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>63</v>
       </c>
@@ -19178,7 +19179,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="188" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>63</v>
       </c>
@@ -19697,7 +19698,7 @@
       <c r="AE192" s="3"/>
       <c r="AK192" s="5"/>
     </row>
-    <row r="193" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>63</v>
       </c>
@@ -39283,7 +39284,13 @@
       <c r="H1843" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AU197" xr:uid="{5695F443-BC3D-48D0-8CD1-D8C4D00277A1}"/>
+  <autoFilter ref="A1:AU197" xr:uid="{5695F443-BC3D-48D0-8CD1-D8C4D00277A1}">
+    <filterColumn colId="4">
+      <filters>
+        <dateGroupItem year="2026" month="2" dateTimeGrouping="month"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="B1:B1823 B1825:B1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
@@ -39297,7 +39304,7 @@
   <dimension ref="A2:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -39322,7 +39329,7 @@
       </c>
       <c r="B3" s="11">
         <f>SUBTOTAL(9,Planilha1!K1:K1825)</f>
-        <v>1676393.95</v>
+        <v>370322.74999999988</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -39337,7 +39344,7 @@
       </c>
       <c r="B4" s="9">
         <f>SUBTOTAL(9,Planilha1!L1:L1820)</f>
-        <v>277307.88</v>
+        <v>67750.310000000012</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -39352,7 +39359,7 @@
       </c>
       <c r="B5" s="12">
         <f>SUBTOTAL(9,Planilha1!M1:M1821)</f>
-        <v>2570261.6015046285</v>
+        <v>28196.620000000006</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -39367,7 +39374,7 @@
       </c>
       <c r="B6" s="10">
         <f>SUBTOTAL(3,Planilha1!D2:D1821)</f>
-        <v>196</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
         <v>214</v>
@@ -39382,7 +39389,7 @@
       </c>
       <c r="B7" s="13">
         <f>B3/B6</f>
-        <v>8553.0303571428576</v>
+        <v>8612.1569767441833</v>
       </c>
       <c r="D7" t="s">
         <v>217</v>
@@ -39397,7 +39404,7 @@
       </c>
       <c r="B8" s="13">
         <f>B3/B4</f>
-        <v>6.0452445491271289</v>
+        <v>5.4659934397348122</v>
       </c>
       <c r="D8" t="s">
         <v>216</v>
@@ -39412,7 +39419,7 @@
       </c>
       <c r="B9" s="13">
         <f>B3/B5</f>
-        <v>0.65222697526922579</v>
+        <v>13.133586578816887</v>
       </c>
       <c r="D9" t="s">
         <v>215</v>

</xml_diff>

<commit_message>
Força atualização cache JS
</commit_message>
<xml_diff>
--- a/excel/PEDIDOS_2026.xlsx
+++ b/excel/PEDIDOS_2026.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USUARIOS\ADM05\Documents\dashboard_tv\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DCA4043-6CA2-4C5C-8826-49C040B42CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A0A9D45-05F6-4727-96BC-0A5BA5D63FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" xr2:uid="{C1828F10-D84A-418A-AAF0-1B51BFAF300A}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3515" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3615" uniqueCount="226">
   <si>
     <t>Empresa/Filial</t>
   </si>
@@ -1110,8 +1110,8 @@
   <dimension ref="A1:AU1843"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N160" sqref="N160"/>
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:AU213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -20828,109 +20828,575 @@
       <c r="AK205" s="5"/>
     </row>
     <row r="206" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="B206" s="1"/>
-      <c r="E206" s="2"/>
-      <c r="F206" s="3"/>
-      <c r="G206" s="3"/>
-      <c r="H206" s="3"/>
-      <c r="I206" s="3"/>
-      <c r="K206" s="3"/>
-      <c r="L206" s="3"/>
-      <c r="X206" s="4"/>
+      <c r="A206" t="s">
+        <v>47</v>
+      </c>
+      <c r="B206" s="1">
+        <v>38559</v>
+      </c>
+      <c r="C206" t="s">
+        <v>48</v>
+      </c>
+      <c r="D206" t="s">
+        <v>49</v>
+      </c>
+      <c r="E206" s="2">
+        <v>46066</v>
+      </c>
+      <c r="F206" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G206" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="H206" s="3">
+        <v>33350</v>
+      </c>
+      <c r="I206" s="3">
+        <v>33350</v>
+      </c>
+      <c r="J206">
+        <v>0</v>
+      </c>
+      <c r="K206" s="3">
+        <v>38352.5</v>
+      </c>
+      <c r="L206" s="3">
+        <v>5077.5</v>
+      </c>
+      <c r="M206" s="3">
+        <v>3239.45</v>
+      </c>
+      <c r="N206" t="s">
+        <v>52</v>
+      </c>
+      <c r="O206" t="s">
+        <v>53</v>
+      </c>
+      <c r="P206" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q206" t="s">
+        <v>53</v>
+      </c>
+      <c r="R206" t="s">
+        <v>54</v>
+      </c>
+      <c r="S206" t="s">
+        <v>54</v>
+      </c>
+      <c r="T206" t="s">
+        <v>55</v>
+      </c>
+      <c r="U206">
+        <v>126</v>
+      </c>
+      <c r="V206" t="s">
+        <v>56</v>
+      </c>
+      <c r="W206" t="s">
+        <v>95</v>
+      </c>
+      <c r="X206" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y206" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="207" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="B207" s="1"/>
-      <c r="E207" s="2"/>
-      <c r="G207" s="3"/>
-      <c r="H207" s="3"/>
-      <c r="I207" s="3"/>
-      <c r="K207" s="3"/>
-      <c r="L207" s="3"/>
+      <c r="A207" t="s">
+        <v>63</v>
+      </c>
+      <c r="B207" s="1">
+        <v>0</v>
+      </c>
+      <c r="C207">
+        <v>0</v>
+      </c>
+      <c r="D207" s="3">
+        <v>5077.5</v>
+      </c>
+      <c r="E207" s="2">
+        <v>0</v>
+      </c>
+      <c r="F207">
+        <v>0</v>
+      </c>
+      <c r="G207" s="3">
+        <v>2500</v>
+      </c>
+      <c r="H207" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I207" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J207" t="s">
+        <v>148</v>
+      </c>
+      <c r="K207" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="L207" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="M207" s="3">
+        <v>46066.471296296295</v>
+      </c>
+      <c r="Q207" t="s">
+        <v>54</v>
+      </c>
+      <c r="R207">
+        <v>0</v>
+      </c>
+      <c r="T207" t="s">
+        <v>54</v>
+      </c>
+      <c r="U207" t="s">
+        <v>54</v>
+      </c>
+      <c r="V207">
+        <v>8478</v>
+      </c>
+      <c r="W207" t="s">
+        <v>55</v>
+      </c>
       <c r="X207" s="4"/>
       <c r="AE207" s="3"/>
       <c r="AK207" s="5"/>
     </row>
     <row r="208" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="B208" s="1"/>
-      <c r="E208" s="2"/>
-      <c r="F208" s="3"/>
-      <c r="G208" s="3"/>
-      <c r="H208" s="3"/>
-      <c r="I208" s="3"/>
-      <c r="K208" s="3"/>
-      <c r="L208" s="3"/>
-      <c r="X208" s="4"/>
+      <c r="A208" t="s">
+        <v>47</v>
+      </c>
+      <c r="B208" s="1">
+        <v>38560</v>
+      </c>
+      <c r="C208" t="s">
+        <v>48</v>
+      </c>
+      <c r="D208" t="s">
+        <v>49</v>
+      </c>
+      <c r="E208" s="2">
+        <v>46066</v>
+      </c>
+      <c r="F208" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G208" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="H208" s="3">
+        <v>33350</v>
+      </c>
+      <c r="I208" s="3">
+        <v>33350</v>
+      </c>
+      <c r="J208">
+        <v>0</v>
+      </c>
+      <c r="K208" s="3">
+        <v>38352.5</v>
+      </c>
+      <c r="L208" s="3">
+        <v>5077.5</v>
+      </c>
+      <c r="M208" s="3">
+        <v>3239.45</v>
+      </c>
+      <c r="N208" t="s">
+        <v>52</v>
+      </c>
+      <c r="O208" t="s">
+        <v>53</v>
+      </c>
+      <c r="P208" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q208" t="s">
+        <v>53</v>
+      </c>
+      <c r="R208" t="s">
+        <v>54</v>
+      </c>
+      <c r="S208" t="s">
+        <v>54</v>
+      </c>
+      <c r="T208" t="s">
+        <v>55</v>
+      </c>
+      <c r="U208">
+        <v>126</v>
+      </c>
+      <c r="V208" t="s">
+        <v>56</v>
+      </c>
+      <c r="W208" t="s">
+        <v>95</v>
+      </c>
+      <c r="X208" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y208" t="s">
+        <v>62</v>
+      </c>
       <c r="AB208" s="3"/>
       <c r="AE208" s="3"/>
       <c r="AK208" s="5"/>
     </row>
-    <row r="209" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B209" s="1"/>
-      <c r="E209" s="2"/>
-      <c r="G209" s="3"/>
-      <c r="H209" s="3"/>
-      <c r="I209" s="3"/>
-      <c r="K209" s="3"/>
-      <c r="L209" s="3"/>
+    <row r="209" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>63</v>
+      </c>
+      <c r="B209" s="1">
+        <v>0</v>
+      </c>
+      <c r="C209">
+        <v>0</v>
+      </c>
+      <c r="D209" s="3">
+        <v>5077.5</v>
+      </c>
+      <c r="E209" s="2">
+        <v>0</v>
+      </c>
+      <c r="F209">
+        <v>0</v>
+      </c>
+      <c r="G209" s="3">
+        <v>2500</v>
+      </c>
+      <c r="H209" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I209" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J209" t="s">
+        <v>148</v>
+      </c>
+      <c r="K209" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="L209" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="M209" s="3">
+        <v>46066.472291666665</v>
+      </c>
+      <c r="Q209" t="s">
+        <v>54</v>
+      </c>
+      <c r="R209">
+        <v>0</v>
+      </c>
+      <c r="T209" t="s">
+        <v>54</v>
+      </c>
+      <c r="U209" t="s">
+        <v>54</v>
+      </c>
+      <c r="V209">
+        <v>8478</v>
+      </c>
+      <c r="W209" t="s">
+        <v>55</v>
+      </c>
       <c r="X209" s="4"/>
       <c r="Z209" s="3"/>
       <c r="AE209" s="3"/>
       <c r="AK209" s="5"/>
     </row>
-    <row r="210" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B210" s="1"/>
-      <c r="D210" s="3"/>
-      <c r="E210" s="2"/>
-      <c r="G210" s="3"/>
-      <c r="H210" s="3"/>
-      <c r="I210" s="3"/>
-      <c r="K210" s="3"/>
-      <c r="L210" s="3"/>
-      <c r="X210" s="4"/>
+    <row r="210" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>47</v>
+      </c>
+      <c r="B210" s="1">
+        <v>38561</v>
+      </c>
+      <c r="C210" t="s">
+        <v>48</v>
+      </c>
+      <c r="D210" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E210" s="2">
+        <v>46066</v>
+      </c>
+      <c r="F210" t="s">
+        <v>147</v>
+      </c>
+      <c r="G210" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="H210" s="3">
+        <v>33350</v>
+      </c>
+      <c r="I210" s="3">
+        <v>33350</v>
+      </c>
+      <c r="J210">
+        <v>0</v>
+      </c>
+      <c r="K210" s="3">
+        <v>38352.5</v>
+      </c>
+      <c r="L210" s="3">
+        <v>5077.5</v>
+      </c>
+      <c r="M210" s="3">
+        <v>3239.45</v>
+      </c>
+      <c r="N210" t="s">
+        <v>52</v>
+      </c>
+      <c r="O210" t="s">
+        <v>53</v>
+      </c>
+      <c r="P210" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q210" t="s">
+        <v>53</v>
+      </c>
+      <c r="R210" t="s">
+        <v>54</v>
+      </c>
+      <c r="S210" t="s">
+        <v>54</v>
+      </c>
+      <c r="T210" t="s">
+        <v>55</v>
+      </c>
+      <c r="U210">
+        <v>126</v>
+      </c>
+      <c r="V210" t="s">
+        <v>56</v>
+      </c>
+      <c r="W210" t="s">
+        <v>95</v>
+      </c>
+      <c r="X210" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y210" t="s">
+        <v>62</v>
+      </c>
       <c r="Z210" s="3"/>
       <c r="AB210" s="3"/>
       <c r="AE210" s="3"/>
       <c r="AK210" s="5"/>
     </row>
-    <row r="211" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B211" s="1"/>
-      <c r="E211" s="2"/>
-      <c r="G211" s="3"/>
-      <c r="H211" s="3"/>
-      <c r="I211" s="3"/>
-      <c r="K211" s="3"/>
-      <c r="L211" s="3"/>
+    <row r="211" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>63</v>
+      </c>
+      <c r="B211" s="1">
+        <v>0</v>
+      </c>
+      <c r="C211">
+        <v>0</v>
+      </c>
+      <c r="D211" s="3">
+        <v>5077.5</v>
+      </c>
+      <c r="E211" s="2">
+        <v>0</v>
+      </c>
+      <c r="F211">
+        <v>0</v>
+      </c>
+      <c r="G211" s="3">
+        <v>2500</v>
+      </c>
+      <c r="H211" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I211" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J211" t="s">
+        <v>148</v>
+      </c>
+      <c r="K211" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="L211" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="M211" s="3">
+        <v>46066.473506944443</v>
+      </c>
+      <c r="Q211" t="s">
+        <v>54</v>
+      </c>
+      <c r="R211">
+        <v>0</v>
+      </c>
+      <c r="T211" t="s">
+        <v>54</v>
+      </c>
+      <c r="U211" t="s">
+        <v>54</v>
+      </c>
+      <c r="V211">
+        <v>8478</v>
+      </c>
+      <c r="W211" t="s">
+        <v>55</v>
+      </c>
       <c r="X211" s="4"/>
       <c r="Z211" s="3"/>
       <c r="AE211" s="3"/>
       <c r="AK211" s="5"/>
     </row>
-    <row r="212" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B212" s="1"/>
-      <c r="E212" s="2"/>
-      <c r="H212" s="3"/>
-      <c r="I212" s="3"/>
-      <c r="K212" s="3"/>
-      <c r="L212" s="3"/>
-      <c r="X212" s="4"/>
+    <row r="212" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>47</v>
+      </c>
+      <c r="B212" s="1">
+        <v>38562</v>
+      </c>
+      <c r="C212" t="s">
+        <v>48</v>
+      </c>
+      <c r="D212" t="s">
+        <v>49</v>
+      </c>
+      <c r="E212" s="2">
+        <v>46066</v>
+      </c>
+      <c r="F212" t="s">
+        <v>147</v>
+      </c>
+      <c r="G212" t="s">
+        <v>89</v>
+      </c>
+      <c r="H212" s="3">
+        <v>33350</v>
+      </c>
+      <c r="I212" s="3">
+        <v>33350</v>
+      </c>
+      <c r="J212">
+        <v>0</v>
+      </c>
+      <c r="K212" s="3">
+        <v>38352.5</v>
+      </c>
+      <c r="L212" s="3">
+        <v>5077.5</v>
+      </c>
+      <c r="M212" s="3">
+        <v>3239.45</v>
+      </c>
+      <c r="N212" t="s">
+        <v>52</v>
+      </c>
+      <c r="O212" t="s">
+        <v>53</v>
+      </c>
+      <c r="P212" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q212" t="s">
+        <v>53</v>
+      </c>
+      <c r="R212" t="s">
+        <v>54</v>
+      </c>
+      <c r="S212" t="s">
+        <v>54</v>
+      </c>
+      <c r="T212" t="s">
+        <v>55</v>
+      </c>
+      <c r="U212">
+        <v>126</v>
+      </c>
+      <c r="V212" t="s">
+        <v>56</v>
+      </c>
+      <c r="W212" t="s">
+        <v>95</v>
+      </c>
+      <c r="X212" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y212" t="s">
+        <v>62</v>
+      </c>
       <c r="Z212" s="3"/>
       <c r="AE212" s="3"/>
       <c r="AK212" s="5"/>
     </row>
-    <row r="213" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B213" s="1"/>
-      <c r="E213" s="2"/>
-      <c r="G213" s="3"/>
-      <c r="H213" s="3"/>
-      <c r="I213" s="3"/>
-      <c r="K213" s="3"/>
-      <c r="L213" s="3"/>
+    <row r="213" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>63</v>
+      </c>
+      <c r="B213" s="1">
+        <v>0</v>
+      </c>
+      <c r="C213">
+        <v>0</v>
+      </c>
+      <c r="D213" s="3">
+        <v>5077.5</v>
+      </c>
+      <c r="E213" s="2">
+        <v>0</v>
+      </c>
+      <c r="F213">
+        <v>0</v>
+      </c>
+      <c r="G213" s="3">
+        <v>2500</v>
+      </c>
+      <c r="H213" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I213" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J213" t="s">
+        <v>148</v>
+      </c>
+      <c r="K213" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="L213" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="M213" s="3">
+        <v>46066.474687499998</v>
+      </c>
+      <c r="Q213" t="s">
+        <v>54</v>
+      </c>
+      <c r="R213">
+        <v>0</v>
+      </c>
+      <c r="T213" t="s">
+        <v>54</v>
+      </c>
+      <c r="U213" t="s">
+        <v>54</v>
+      </c>
+      <c r="V213">
+        <v>8478</v>
+      </c>
+      <c r="W213" t="s">
+        <v>55</v>
+      </c>
       <c r="X213" s="4"/>
       <c r="Z213" s="3"/>
       <c r="AE213" s="3"/>
       <c r="AK213" s="5"/>
     </row>
-    <row r="214" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B214" s="1"/>
       <c r="E214" s="2"/>
       <c r="H214" s="3"/>
@@ -20942,7 +21408,7 @@
       <c r="AE214" s="3"/>
       <c r="AK214" s="5"/>
     </row>
-    <row r="215" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B215" s="3"/>
       <c r="E215" s="2"/>
       <c r="G215" s="3"/>
@@ -20954,7 +21420,7 @@
       <c r="AE215" s="3"/>
       <c r="AK215" s="5"/>
     </row>
-    <row r="216" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B216" s="1"/>
       <c r="C216" s="3"/>
       <c r="E216" s="2"/>
@@ -20965,7 +21431,7 @@
       <c r="L216" s="3"/>
       <c r="X216" s="4"/>
     </row>
-    <row r="217" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B217" s="3"/>
       <c r="E217" s="2"/>
       <c r="G217" s="3"/>
@@ -20978,7 +21444,7 @@
       <c r="AE217" s="3"/>
       <c r="AK217" s="5"/>
     </row>
-    <row r="218" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B218" s="1"/>
       <c r="E218" s="2"/>
       <c r="H218" s="3"/>
@@ -20990,14 +21456,14 @@
       <c r="AE218" s="3"/>
       <c r="AK218" s="5"/>
     </row>
-    <row r="219" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B219" s="1"/>
       <c r="D219" s="3"/>
       <c r="E219" s="2"/>
       <c r="G219" s="3"/>
       <c r="X219" s="4"/>
     </row>
-    <row r="220" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B220" s="1"/>
       <c r="E220" s="2"/>
       <c r="H220" s="3"/>
@@ -21009,7 +21475,7 @@
       <c r="AE220" s="3"/>
       <c r="AK220" s="5"/>
     </row>
-    <row r="221" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B221" s="1"/>
       <c r="E221" s="2"/>
       <c r="F221" s="3"/>
@@ -21023,7 +21489,7 @@
       <c r="AE221" s="3"/>
       <c r="AK221" s="5"/>
     </row>
-    <row r="222" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B222" s="3"/>
       <c r="E222" s="2"/>
       <c r="G222" s="3"/>
@@ -21035,7 +21501,7 @@
       <c r="AE222" s="3"/>
       <c r="AK222" s="5"/>
     </row>
-    <row r="223" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B223" s="1"/>
       <c r="D223" s="3"/>
       <c r="E223" s="2"/>
@@ -21045,7 +21511,7 @@
       <c r="K223" s="3"/>
       <c r="X223" s="4"/>
     </row>
-    <row r="224" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B224" s="1"/>
       <c r="E224" s="2"/>
       <c r="G224" s="3"/>
@@ -39806,7 +40272,7 @@
       </c>
       <c r="B3" s="11">
         <f>SUBTOTAL(9,Planilha1!K1:K1825)</f>
-        <v>1748475</v>
+        <v>1901885</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -39821,7 +40287,7 @@
       </c>
       <c r="B4" s="9">
         <f>SUBTOTAL(9,Planilha1!L1:L1820)</f>
-        <v>293017.28000000003</v>
+        <v>313327.28000000003</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -39836,7 +40302,7 @@
       </c>
       <c r="B5" s="12">
         <f>SUBTOTAL(9,Planilha1!M1:M1821)</f>
-        <v>2760199.81054398</v>
+        <v>2957423.5023263879</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -39851,7 +40317,7 @@
       </c>
       <c r="B6" s="10">
         <f>SUBTOTAL(3,Planilha1!D2:D1821)</f>
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="D6" t="s">
         <v>214</v>
@@ -39866,7 +40332,7 @@
       </c>
       <c r="B7" s="13">
         <f>B3/B6</f>
-        <v>8570.9558823529405</v>
+        <v>8971.1556603773588</v>
       </c>
       <c r="D7" t="s">
         <v>217</v>
@@ -39881,7 +40347,7 @@
       </c>
       <c r="B8" s="13">
         <f>B3/B4</f>
-        <v>5.9671395489030541</v>
+        <v>6.0699630112003007</v>
       </c>
       <c r="D8" t="s">
         <v>216</v>
@@ -39896,7 +40362,7 @@
       </c>
       <c r="B9" s="13">
         <f>B3/B5</f>
-        <v>0.63345957539769948</v>
+        <v>0.64308848513035988</v>
       </c>
       <c r="D9" t="s">
         <v>215</v>

</xml_diff>

<commit_message>
Atualização painel 2026-02-19 09:33
</commit_message>
<xml_diff>
--- a/excel/PEDIDOS_2026.xlsx
+++ b/excel/PEDIDOS_2026.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USUARIOS\ADM05\Documents\dashboard_tv\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B17BF2-E0B4-4150-864E-0033DA931FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65F2FF3-878D-400B-895F-DE6065885992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" xr2:uid="{C1828F10-D84A-418A-AAF0-1B51BFAF300A}"/>
   </bookViews>
@@ -1146,8 +1146,8 @@
   <dimension ref="A1:AU1843"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A183" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B191" sqref="B191"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>

</xml_diff>